<commit_message>
rename method, fix bug
</commit_message>
<xml_diff>
--- a/dulieu/datPhongOutput.xlsx
+++ b/dulieu/datPhongOutput.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>ID Đặt Hàng</t>
   </si>
@@ -38,31 +38,49 @@
     <t>1</t>
   </si>
   <si>
-    <t>2025-07-23T17:04:35.939278</t>
-  </si>
-  <si>
-    <t>2028-11-11T00:00</t>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2025-07-24T15:21:07.190196</t>
+  </si>
+  <si>
+    <t>2025-08-01T00:00</t>
+  </si>
+  <si>
+    <t>không</t>
+  </si>
+  <si>
+    <t>DA_THANH_TOAN</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2025-07-24T15:22:00.809863</t>
+  </si>
+  <si>
+    <t>2025-11-11T00:00</t>
   </si>
   <si>
     <t>ko</t>
   </si>
   <si>
-    <t>DA_THANH_TOAN</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>2025-07-23T17:13:27.540578</t>
-  </si>
-  <si>
-    <t>2025-11-11T00:00</t>
-  </si>
-  <si>
-    <t>3sfd</t>
-  </si>
-  <si>
-    <t>CHUA_THANH_TOAN</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2025-07-24T16:02:39.798387</t>
+  </si>
+  <si>
+    <t>2025-07-24T16:06:10.862699</t>
+  </si>
+  <si>
+    <t>2026-11-11T00:00</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -107,7 +125,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -119,7 +137,7 @@
     <col min="4" max="4" width="29.25" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="18.8125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="6.69140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="19.703125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="17.1875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -153,42 +171,88 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
-        <v>16</v>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>